<commit_message>
river rec labels revision
</commit_message>
<xml_diff>
--- a/src/dams_mcda/www/DecisionMatrices_All.xlsx
+++ b/src/dams_mcda/www/DecisionMatrices_All.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Beatrice2\NEST_ELF\Future_of_Dams\MCDA\Dam Decision Support Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Beatrice2\R_ELF\R_NEST\MCDA_App_Shiny\MCDA_06262019\src\dams_mcda\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20235" windowHeight="7050" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20235" windowHeight="7050" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="10" r:id="rId1"/>
     <sheet name="West Enfield" sheetId="3" r:id="rId2"/>
     <sheet name="Medway" sheetId="4" r:id="rId3"/>
-    <sheet name="MillinocketQuakish" sheetId="5" r:id="rId4"/>
-    <sheet name="East Millinocket" sheetId="6" r:id="rId5"/>
-    <sheet name="North Twin" sheetId="7" r:id="rId6"/>
-    <sheet name="Dolby" sheetId="8" r:id="rId7"/>
+    <sheet name="East Millinocket" sheetId="6" r:id="rId4"/>
+    <sheet name="Dolby" sheetId="8" r:id="rId5"/>
+    <sheet name="MillinocketQuakish" sheetId="5" r:id="rId6"/>
+    <sheet name="North Twin" sheetId="7" r:id="rId7"/>
     <sheet name="Millinocket Lake" sheetId="9" r:id="rId8"/>
     <sheet name="Ripogenus" sheetId="2" r:id="rId9"/>
     <sheet name="METADATA" sheetId="1" r:id="rId10"/>
@@ -109,9 +109,6 @@
     <t>See Roy et al. (2018)</t>
   </si>
   <si>
-    <t>Estimated as possible upstream sea-run fish (Atlantic salmon, Alewife, Blueback herring, American eel) habitat area calculated using functional habitat units (Roy et al., 2019).</t>
-  </si>
-  <si>
     <t>https://www.pnas.org/content/pnas/suppl/2018/10/31/1807437115.DCSupplemental/pnas.1807437115.sapp.pdf</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>square km</t>
   </si>
   <si>
-    <t>Estimated downstream area of river that may increase or decrease with a dam decision alternative, combines functional area for whitewater and flatwater recreation defined by Roy et al. (2019).</t>
-  </si>
-  <si>
     <t>Number of Properties Impacted</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
   </si>
   <si>
     <t xml:space="preserve">Reservoir storage </t>
-  </si>
-  <si>
-    <t>Estimated storage potential of the reservoir based on its volume, calculated from max depth to the hydraulic height of the damand the base of the dam (Roy et al., 2019)</t>
   </si>
   <si>
     <t>Indigenous Lifeways</t>
@@ -269,9 +260,6 @@
     <t>unitless</t>
   </si>
   <si>
-    <t>A proxy for safety based on the State hazard rating, which indicates the potential for downstream property damage, injury, and death in the case of dam breach (Roy et al., 2019).</t>
-  </si>
-  <si>
     <t>p.5, eq. 12</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
   </si>
   <si>
     <t>no. properties</t>
-  </si>
-  <si>
-    <t>Estimated number of properties impacted by the decision alternative, based on potential changes in viewshed or property value (Roy et al., 2019).</t>
   </si>
   <si>
     <t>p.4, eq. 8</t>
@@ -309,9 +294,6 @@
   </si>
   <si>
     <t>User</t>
-  </si>
-  <si>
-    <t>For NOAA workshop, calculated as the non-weighted average of user input values.</t>
   </si>
   <si>
     <t>Rating to convey the importance of the dam for preserving/restoring the industrial historical value of the infrastructure.</t>
@@ -524,12 +506,6 @@
     <t>*1 GW = 1000 MW, so to convert from GW to MW, multiply the value by 1,000. To convert from MW to GW, divide by 1,000.</t>
   </si>
   <si>
-    <t>Set at 5 for remove dam, 2 for improve fish passage, and 0 for all other decision alternatives because having a free-flowing Penobscot River is crucial to Penobscot Nation cultural traditions and lifeways, and Penobscot Nation is defined as a disadvantaged group in this context.</t>
-  </si>
-  <si>
-    <t>Set at 5 for remove dam, 2 for improve fish passage, and 0 for all other decision alternatives because having a free-flowing Penobscot River is crucial to Penobscot Nation cultural traditions and lifeways</t>
-  </si>
-  <si>
     <t>0 -16</t>
   </si>
   <si>
@@ -553,6 +529,30 @@
   <si>
     <t>Annual CO2 emissions reduction - based on avoiding the Maine electricity generation mix, life cycle for coal and gas, point-source for other fossil fuels, subtracting life cycle for hydro diversion from Figure 6 in Song et al. (2018). Where dams are diversion-style, 0.180 is used as the GHG emissions avoided (kgCO2eq/kWh) value.</t>
   </si>
+  <si>
+    <t>Estimated as possible upstream sea-run fish (Atlantic salmon, Alewife, Blueback herring, American eel) habitat area calculated using functional habitat units (Roy et al., 2018).</t>
+  </si>
+  <si>
+    <t>Estimated storage potential of the reservoir based on its volume, calculated from max depth to the hydraulic height of the damand the base of the dam (Roy et al., 2018)</t>
+  </si>
+  <si>
+    <t>A proxy for safety based on the State hazard rating, which indicates the potential for downstream property damage, injury, and death in the case of dam breach (Roy et al., 2018).</t>
+  </si>
+  <si>
+    <t>Estimated number of properties impacted by the decision alternative, based on potential changes in viewshed or property value (Roy et al., 2018).</t>
+  </si>
+  <si>
+    <t>Averaged pre-survey input from all Penobscot Nation participants to be used for all decision alternatives because having a free-flowing Penobscot River is crucial to Penobscot Nation cultural traditions and lifeways.</t>
+  </si>
+  <si>
+    <t>Calculated as the average of municipal and Penobscot Nation participant pre-survey input values.</t>
+  </si>
+  <si>
+    <t>Calculated as the non-weighted average of participant pre-survey input values.</t>
+  </si>
+  <si>
+    <t>Estimated downstream area of river that may increase or decrease with a dam decision alternative, represents functional area for whitewater recreation defined by Roy et al. (2018).</t>
+  </si>
 </sst>
 </file>
 
@@ -560,7 +560,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -958,9 +958,6 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -969,14 +966,17 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1268,17 +1268,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1293,8 +1293,8 @@
   </sheetPr>
   <dimension ref="A1:AA1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1361,28 +1361,28 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1403,33 +1403,33 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>30</v>
+      <c r="E3" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1452,31 +1452,31 @@
     </row>
     <row r="4" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>37</v>
+      <c r="E4" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1499,31 +1499,31 @@
     </row>
     <row r="5" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1546,31 +1546,31 @@
     </row>
     <row r="6" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="H6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="31" t="s">
         <v>54</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>57</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1593,31 +1593,31 @@
     </row>
     <row r="7" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="H7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="I7" s="31" t="s">
         <v>60</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>63</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1640,31 +1640,31 @@
     </row>
     <row r="8" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1687,31 +1687,31 @@
     </row>
     <row r="9" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="G9" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1734,31 +1734,31 @@
     </row>
     <row r="10" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>70</v>
+      <c r="E10" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1781,31 +1781,31 @@
     </row>
     <row r="11" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>75</v>
+      <c r="E11" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1828,28 +1828,28 @@
     </row>
     <row r="12" spans="1:27" s="40" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="35"/>
@@ -1873,31 +1873,31 @@
     </row>
     <row r="13" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>164</v>
+        <v>155</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>156</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1920,31 +1920,31 @@
     </row>
     <row r="14" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1967,31 +1967,31 @@
     </row>
     <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>163</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2014,31 +2014,31 @@
     </row>
     <row r="16" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>162</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2061,31 +2061,31 @@
     </row>
     <row r="17" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>163</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2108,31 +2108,31 @@
     </row>
     <row r="18" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="26" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>163</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2153,33 +2153,33 @@
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
     </row>
-    <row r="19" spans="1:27" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2200,33 +2200,33 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
     </row>
-    <row r="20" spans="1:27" s="40" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" s="40" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I20" s="39" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
@@ -2249,31 +2249,31 @@
     </row>
     <row r="21" spans="1:27" s="40" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
@@ -2296,31 +2296,31 @@
     </row>
     <row r="22" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2343,31 +2343,31 @@
     </row>
     <row r="23" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>103</v>
-      </c>
       <c r="E23" s="15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2390,31 +2390,31 @@
     </row>
     <row r="24" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -2437,31 +2437,31 @@
     </row>
     <row r="25" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>44</v>
-      </c>
       <c r="G25" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -2482,33 +2482,33 @@
       <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
     </row>
-    <row r="26" spans="1:27" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2531,31 +2531,31 @@
     </row>
     <row r="27" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I27" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2578,31 +2578,31 @@
     </row>
     <row r="28" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F29" s="24"/>
       <c r="H29" s="23"/>
@@ -31054,6 +31054,7 @@
     <hyperlink ref="F28" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -31062,8 +31063,8 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:F15"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31149,7 +31150,7 @@
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50">
         <v>11.7</v>
@@ -31164,12 +31165,12 @@
         <v>11.7</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="50">
         <v>0</v>
@@ -31189,7 +31190,7 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
         <v>948.97299999999996</v>
@@ -31209,7 +31210,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
         <v>3</v>
@@ -31227,9 +31228,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -31249,7 +31250,7 @@
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="45">
         <v>73</v>
@@ -31269,21 +31270,21 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="66">
+        <v>33</v>
+      </c>
+      <c r="B9" s="65">
         <f>9612.21085822381/1000</f>
         <v>9.6122108582238113</v>
       </c>
-      <c r="C9" s="66">
+      <c r="C9" s="65">
         <f t="shared" ref="C9:E9" si="0">9612.21085822381/1000</f>
         <v>9.6122108582238113</v>
       </c>
-      <c r="D9" s="66">
+      <c r="D9" s="65">
         <f t="shared" si="0"/>
         <v>9.6122108582238113</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="65">
         <f t="shared" si="0"/>
         <v>9.6122108582238113</v>
       </c>
@@ -31293,133 +31294,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="C11" s="65">
-        <v>2.1666666669999999</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2</v>
-      </c>
-      <c r="E11" s="65">
-        <v>2.3333333330000001</v>
-      </c>
-      <c r="F11" s="65">
-        <v>2.1666666669999999</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3.2</v>
-      </c>
-      <c r="C12" s="65">
-        <v>3.2</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E12" s="65">
-        <v>3</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3.8</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>1.5</v>
-      </c>
-      <c r="C13" s="65">
-        <v>3</v>
-      </c>
-      <c r="D13" s="65">
-        <v>1.8333333329999999</v>
-      </c>
-      <c r="E13" s="65">
-        <v>2.8333333330000001</v>
-      </c>
-      <c r="F13" s="65">
-        <v>4.8</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>1.4</v>
-      </c>
-      <c r="C14" s="65">
-        <v>3.2</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E14" s="65">
-        <v>2.8</v>
-      </c>
-      <c r="F14" s="65">
-        <v>4.25</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -34362,8 +34303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34449,7 +34390,7 @@
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50">
         <v>0</v>
@@ -34464,12 +34405,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="50">
         <v>0</v>
@@ -34489,7 +34430,7 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
         <v>246</v>
@@ -34509,7 +34450,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
         <v>3</v>
@@ -34529,7 +34470,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -34549,7 +34490,7 @@
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="45">
         <v>28</v>
@@ -34569,21 +34510,21 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="67">
+        <v>33</v>
+      </c>
+      <c r="B9" s="66">
         <f>5058.83186163302/1000</f>
         <v>5.0588318616330197</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="66">
         <f>8676.48487896361/1000</f>
         <v>8.6764848789636115</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="66">
         <f>5058.83186163302/1000</f>
         <v>5.0588318616330197</v>
       </c>
-      <c r="E9" s="67">
+      <c r="E9" s="66">
         <f>8676.48487896361/1000</f>
         <v>8.6764848789636115</v>
       </c>
@@ -34593,133 +34534,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="52">
-        <v>3.4285714289999998</v>
-      </c>
-      <c r="C11" s="64">
-        <v>3</v>
-      </c>
-      <c r="D11" s="52">
-        <v>3.1428571430000001</v>
-      </c>
-      <c r="E11" s="65">
-        <v>2.8333333330000001</v>
-      </c>
-      <c r="F11" s="65">
-        <v>2.3333333330000001</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3.3333333330000001</v>
-      </c>
-      <c r="C12" s="65">
-        <v>3.1666666669999999</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="65">
-        <v>2.8333333330000001</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3.8333333330000001</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>1.5555555560000001</v>
-      </c>
-      <c r="C13" s="65">
-        <v>2.875</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2.111111111</v>
-      </c>
-      <c r="E13" s="65">
-        <v>2.6666666669999999</v>
-      </c>
-      <c r="F13" s="65">
-        <v>4.5714285710000002</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>1.6666666670000001</v>
-      </c>
-      <c r="C14" s="65">
-        <v>3.3333333330000001</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.3333333330000001</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3</v>
-      </c>
-      <c r="F14" s="65">
-        <v>4</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -37659,11 +37540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37735,21 +37616,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50">
         <v>0.29859999999999998</v>
@@ -37763,57 +37644,53 @@
       <c r="E3" s="50">
         <v>0.29859999999999998</v>
       </c>
-      <c r="F3" s="59" t="s">
-        <v>157</v>
+      <c r="F3" s="60" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="54">
-        <f t="shared" ref="B4:E4" si="0">9869/100000</f>
-        <v>9.869E-2</v>
-      </c>
-      <c r="C4" s="54">
-        <f t="shared" si="0"/>
-        <v>9.869E-2</v>
-      </c>
-      <c r="D4" s="54">
-        <f t="shared" si="0"/>
-        <v>9.869E-2</v>
-      </c>
-      <c r="E4" s="54">
-        <f t="shared" si="0"/>
-        <v>9.869E-2</v>
-      </c>
-      <c r="F4" s="55">
+        <v>24</v>
+      </c>
+      <c r="B4" s="50">
+        <v>0</v>
+      </c>
+      <c r="C4" s="50">
+        <v>0</v>
+      </c>
+      <c r="D4" s="50">
+        <v>0</v>
+      </c>
+      <c r="E4" s="50">
+        <v>0</v>
+      </c>
+      <c r="F4" s="50">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
-        <v>1657.029</v>
+        <v>406.4</v>
       </c>
       <c r="C5" s="50">
-        <v>1969.8309999999999</v>
+        <v>470.74299999999999</v>
       </c>
       <c r="D5" s="50">
-        <v>1657.029</v>
+        <v>1897.182</v>
       </c>
       <c r="E5" s="50">
-        <v>1969.8309999999999</v>
+        <v>1961.5250000000001</v>
       </c>
       <c r="F5" s="50">
-        <v>215.15199999999999</v>
+        <v>168.458</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
         <v>1</v>
@@ -37833,7 +37710,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -37848,24 +37725,24 @@
         <v>0</v>
       </c>
       <c r="F7" s="50">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="45">
-        <v>203</v>
+        <v>38</v>
       </c>
       <c r="C8" s="45">
-        <v>203</v>
+        <v>38</v>
       </c>
       <c r="D8" s="45">
-        <v>203</v>
+        <v>60</v>
       </c>
       <c r="E8" s="45">
-        <v>203</v>
+        <v>60</v>
       </c>
       <c r="F8" s="50">
         <v>0</v>
@@ -37873,19 +37750,19 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="68">
-        <v>26.69620857</v>
-      </c>
-      <c r="C9" s="68">
-        <v>26.69620857</v>
+        <v>33</v>
+      </c>
+      <c r="B9" s="67">
+        <v>6.782771221</v>
+      </c>
+      <c r="C9" s="67">
+        <v>6.782771221</v>
       </c>
       <c r="D9" s="68">
-        <v>26.69620857</v>
+        <v>10.756990114000001</v>
       </c>
       <c r="E9" s="68">
-        <v>26.69620857</v>
+        <v>10.756990114000001</v>
       </c>
       <c r="F9" s="50">
         <v>0</v>
@@ -37893,133 +37770,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3.6</v>
-      </c>
-      <c r="C11" s="65">
-        <v>2.6</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E11" s="65">
-        <v>2.6</v>
-      </c>
-      <c r="F11" s="65">
-        <v>2</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3.4</v>
-      </c>
-      <c r="C12" s="65">
-        <v>2.6</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E12" s="65">
-        <v>2.6</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3.2</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>1.4</v>
-      </c>
-      <c r="C13" s="65">
-        <v>3.2</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2</v>
-      </c>
-      <c r="E13" s="65">
-        <v>3</v>
-      </c>
-      <c r="F13" s="65">
-        <v>4.8</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>1.75</v>
-      </c>
-      <c r="C14" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.25</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3</v>
-      </c>
-      <c r="F14" s="65">
-        <v>4.25</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -40955,7 +40772,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -40964,7 +40780,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F15"/>
+      <selection activeCell="B10" sqref="B10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -41036,93 +40852,97 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50">
-        <v>0.29859999999999998</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="C3" s="50">
-        <v>0.29859999999999998</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="D3" s="50">
-        <v>0.29859999999999998</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="E3" s="50">
-        <v>0.29859999999999998</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>160</v>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="50">
-        <v>0</v>
-      </c>
-      <c r="C4" s="50">
-        <v>0</v>
-      </c>
-      <c r="D4" s="50">
-        <v>0</v>
-      </c>
-      <c r="E4" s="50">
-        <v>0</v>
-      </c>
-      <c r="F4" s="50">
+        <v>24</v>
+      </c>
+      <c r="B4" s="54">
+        <f t="shared" ref="B4:E4" si="0">33163/100000</f>
+        <v>0.33162999999999998</v>
+      </c>
+      <c r="C4" s="54">
+        <f t="shared" si="0"/>
+        <v>0.33162999999999998</v>
+      </c>
+      <c r="D4" s="54">
+        <f t="shared" si="0"/>
+        <v>0.33162999999999998</v>
+      </c>
+      <c r="E4" s="54">
+        <f t="shared" si="0"/>
+        <v>0.33162999999999998</v>
+      </c>
+      <c r="F4" s="55">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
-        <v>406.4</v>
+        <v>1229.307</v>
       </c>
       <c r="C5" s="50">
-        <v>470.74299999999999</v>
+        <v>1414.53</v>
       </c>
       <c r="D5" s="50">
-        <v>1897.182</v>
+        <v>1229.307</v>
       </c>
       <c r="E5" s="50">
-        <v>1961.5250000000001</v>
+        <v>1414.53</v>
       </c>
       <c r="F5" s="50">
-        <v>168.458</v>
+        <v>319.43299999999999</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -41130,7 +40950,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -41145,24 +40965,24 @@
         <v>0</v>
       </c>
       <c r="F7" s="50">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="45">
-        <v>38</v>
-      </c>
-      <c r="C8" s="45">
-        <v>38</v>
-      </c>
-      <c r="D8" s="45">
-        <v>60</v>
-      </c>
-      <c r="E8" s="45">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="50">
+        <v>98.1</v>
+      </c>
+      <c r="C8" s="50">
+        <v>98.1</v>
+      </c>
+      <c r="D8" s="50">
+        <v>98.1</v>
+      </c>
+      <c r="E8" s="50">
+        <v>98.1</v>
       </c>
       <c r="F8" s="50">
         <v>0</v>
@@ -41170,19 +40990,19 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="68">
-        <v>6.782771221</v>
+        <v>12.88193832</v>
       </c>
       <c r="C9" s="68">
-        <v>6.782771221</v>
-      </c>
-      <c r="D9" s="69">
-        <v>10.756990114000001</v>
-      </c>
-      <c r="E9" s="69">
-        <v>10.756990114000001</v>
+        <v>12.88193832</v>
+      </c>
+      <c r="D9" s="68">
+        <v>12.88193832</v>
+      </c>
+      <c r="E9" s="68">
+        <v>12.88193832</v>
       </c>
       <c r="F9" s="50">
         <v>0</v>
@@ -41190,133 +41010,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="C11" s="65">
-        <v>2.75</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2</v>
-      </c>
-      <c r="E11" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="F11" s="65">
-        <v>2.25</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="C12" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.25</v>
-      </c>
-      <c r="E12" s="65">
-        <v>3</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3.75</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>1.5</v>
-      </c>
-      <c r="C13" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2.25</v>
-      </c>
-      <c r="E13" s="65">
-        <v>3</v>
-      </c>
-      <c r="F13" s="65">
-        <v>4.75</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>1.75</v>
-      </c>
-      <c r="C14" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.25</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3</v>
-      </c>
-      <c r="F14" s="65">
-        <v>4.25</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -44256,11 +44016,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F15"/>
+      <selection activeCell="B10" sqref="B10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44332,57 +44092,57 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50">
-        <v>1.57</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="C3" s="50">
-        <v>1.57</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="D3" s="50">
-        <v>1.57</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="E3" s="50">
-        <v>1.57</v>
-      </c>
-      <c r="F3" s="61" t="s">
-        <v>161</v>
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="54">
-        <f t="shared" ref="B4:E4" si="0">21456/100000</f>
-        <v>0.21456</v>
+        <f t="shared" ref="B4:E4" si="0">9869/100000</f>
+        <v>9.869E-2</v>
       </c>
       <c r="C4" s="54">
         <f t="shared" si="0"/>
-        <v>0.21456</v>
+        <v>9.869E-2</v>
       </c>
       <c r="D4" s="54">
         <f t="shared" si="0"/>
-        <v>0.21456</v>
+        <v>9.869E-2</v>
       </c>
       <c r="E4" s="54">
         <f t="shared" si="0"/>
-        <v>0.21456</v>
+        <v>9.869E-2</v>
       </c>
       <c r="F4" s="55">
         <v>0</v>
@@ -44390,39 +44150,39 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
-        <v>402.8</v>
+        <v>1657.029</v>
       </c>
       <c r="C5" s="50">
-        <v>467.46300000000002</v>
+        <v>1969.8309999999999</v>
       </c>
       <c r="D5" s="50">
-        <v>1880.377</v>
+        <v>1657.029</v>
       </c>
       <c r="E5" s="50">
-        <v>1945.04</v>
+        <v>1969.8309999999999</v>
       </c>
       <c r="F5" s="50">
-        <v>212.08799999999999</v>
+        <v>215.15199999999999</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -44430,7 +44190,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -44445,24 +44205,24 @@
         <v>0</v>
       </c>
       <c r="F7" s="50">
-        <v>589</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="45">
-        <v>47</v>
+        <v>203</v>
       </c>
       <c r="C8" s="45">
-        <v>47</v>
+        <v>203</v>
       </c>
       <c r="D8" s="45">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="E8" s="45">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="F8" s="50">
         <v>0</v>
@@ -44470,20 +44230,19 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="69">
-        <f>8.509949038</f>
-        <v>8.5099490380000002</v>
-      </c>
-      <c r="C9" s="69">
-        <v>8.5099490380000002</v>
-      </c>
-      <c r="D9" s="69">
-        <v>13.426482992</v>
-      </c>
-      <c r="E9" s="69">
-        <v>13.426482992</v>
+        <v>33</v>
+      </c>
+      <c r="B9" s="67">
+        <v>26.69620857</v>
+      </c>
+      <c r="C9" s="67">
+        <v>26.69620857</v>
+      </c>
+      <c r="D9" s="67">
+        <v>26.69620857</v>
+      </c>
+      <c r="E9" s="67">
+        <v>26.69620857</v>
       </c>
       <c r="F9" s="50">
         <v>0</v>
@@ -44491,133 +44250,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3</v>
-      </c>
-      <c r="C11" s="65">
-        <v>4</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E11" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="65">
-        <v>3</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3</v>
-      </c>
-      <c r="C12" s="65">
-        <v>4</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>3</v>
-      </c>
-      <c r="C13" s="65">
-        <v>4</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E13" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F13" s="65">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="C14" s="65">
-        <v>4</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="65">
-        <v>3.5</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -47553,6 +47252,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -47561,7 +47261,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F15"/>
+      <selection activeCell="B10" sqref="B10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -47633,57 +47333,57 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="50">
-        <v>0.32500000000000001</v>
+        <v>1.57</v>
       </c>
       <c r="C3" s="50">
-        <v>0.32500000000000001</v>
+        <v>1.57</v>
       </c>
       <c r="D3" s="50">
-        <v>0.32500000000000001</v>
+        <v>1.57</v>
       </c>
       <c r="E3" s="50">
-        <v>0.32500000000000001</v>
+        <v>1.57</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="54">
-        <f t="shared" ref="B4:E4" si="0">33163/100000</f>
-        <v>0.33162999999999998</v>
+        <f t="shared" ref="B4:E4" si="0">21456/100000</f>
+        <v>0.21456</v>
       </c>
       <c r="C4" s="54">
         <f t="shared" si="0"/>
-        <v>0.33162999999999998</v>
+        <v>0.21456</v>
       </c>
       <c r="D4" s="54">
         <f t="shared" si="0"/>
-        <v>0.33162999999999998</v>
+        <v>0.21456</v>
       </c>
       <c r="E4" s="54">
         <f t="shared" si="0"/>
-        <v>0.33162999999999998</v>
+        <v>0.21456</v>
       </c>
       <c r="F4" s="55">
         <v>0</v>
@@ -47691,27 +47391,27 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
-        <v>1229.307</v>
+        <v>402.8</v>
       </c>
       <c r="C5" s="50">
-        <v>1414.53</v>
+        <v>467.46300000000002</v>
       </c>
       <c r="D5" s="50">
-        <v>1229.307</v>
+        <v>1880.377</v>
       </c>
       <c r="E5" s="50">
-        <v>1414.53</v>
+        <v>1945.04</v>
       </c>
       <c r="F5" s="50">
-        <v>319.43299999999999</v>
+        <v>212.08799999999999</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
         <v>2</v>
@@ -47731,7 +47431,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -47746,24 +47446,24 @@
         <v>0</v>
       </c>
       <c r="F7" s="50">
-        <v>25</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="50">
-        <v>98.1</v>
-      </c>
-      <c r="C8" s="50">
-        <v>98.1</v>
-      </c>
-      <c r="D8" s="50">
-        <v>98.1</v>
-      </c>
-      <c r="E8" s="50">
-        <v>98.1</v>
+        <v>30</v>
+      </c>
+      <c r="B8" s="45">
+        <v>47</v>
+      </c>
+      <c r="C8" s="45">
+        <v>47</v>
+      </c>
+      <c r="D8" s="45">
+        <v>75</v>
+      </c>
+      <c r="E8" s="45">
+        <v>75</v>
       </c>
       <c r="F8" s="50">
         <v>0</v>
@@ -47771,19 +47471,20 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="69">
-        <v>12.88193832</v>
-      </c>
-      <c r="C9" s="69">
-        <v>12.88193832</v>
-      </c>
-      <c r="D9" s="69">
-        <v>12.88193832</v>
-      </c>
-      <c r="E9" s="69">
-        <v>12.88193832</v>
+        <v>33</v>
+      </c>
+      <c r="B9" s="68">
+        <f>8.509949038</f>
+        <v>8.5099490380000002</v>
+      </c>
+      <c r="C9" s="68">
+        <v>8.5099490380000002</v>
+      </c>
+      <c r="D9" s="68">
+        <v>13.426482992</v>
+      </c>
+      <c r="E9" s="68">
+        <v>13.426482992</v>
       </c>
       <c r="F9" s="50">
         <v>0</v>
@@ -47791,133 +47492,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3</v>
-      </c>
-      <c r="C11" s="65">
-        <v>4</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E11" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="65">
-        <v>3</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3</v>
-      </c>
-      <c r="C12" s="65">
-        <v>4</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>2</v>
-      </c>
-      <c r="C13" s="65">
-        <v>4</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E13" s="65">
-        <v>3</v>
-      </c>
-      <c r="F13" s="65">
-        <v>4</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>1.5</v>
-      </c>
-      <c r="C14" s="65">
-        <v>4</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="65">
-        <v>4.5</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+    </row>
+    <row r="16" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -50860,8 +50501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="B3:F15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -50933,21 +50574,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="52">
         <v>0</v>
@@ -50967,7 +50608,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="56">
         <f t="shared" ref="B4:E4" si="0">40583/100000</f>
@@ -50991,7 +50632,7 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="52">
         <v>1</v>
@@ -51011,7 +50652,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="52">
         <v>2</v>
@@ -51031,7 +50672,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="52">
         <v>0</v>
@@ -51051,7 +50692,7 @@
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="52">
         <v>0</v>
@@ -51071,7 +50712,7 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="58">
         <v>0</v>
@@ -51079,10 +50720,10 @@
       <c r="C9" s="52">
         <v>0</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="68">
         <v>9.5859479999999997E-2</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="68">
         <v>9.5859479999999997E-2</v>
       </c>
       <c r="F9" s="52">
@@ -51091,133 +50732,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3</v>
-      </c>
-      <c r="C11" s="65">
-        <v>4</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E11" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F11" s="65">
-        <v>3</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3</v>
-      </c>
-      <c r="C12" s="65">
-        <v>4</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>3</v>
-      </c>
-      <c r="C13" s="65">
-        <v>4</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E13" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F13" s="65">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="C14" s="65">
-        <v>4</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3.5</v>
-      </c>
-      <c r="F14" s="65">
-        <v>3.5</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -54233,21 +53814,21 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="52" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="52" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="50">
         <v>2.2000000000000002</v>
@@ -54262,12 +53843,12 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="57">
         <f t="shared" ref="B4:E4" si="0">1378212/100000</f>
@@ -54291,7 +53872,7 @@
     </row>
     <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="50">
         <v>747</v>
@@ -54311,7 +53892,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="50">
         <v>3</v>
@@ -54331,7 +53912,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="50">
         <v>0</v>
@@ -54351,7 +53932,7 @@
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="45">
         <v>234</v>
@@ -54371,18 +53952,18 @@
     </row>
     <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="69">
+        <v>33</v>
+      </c>
+      <c r="B9" s="68">
         <v>30.727559299999999</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="68">
         <v>30.727559299999999</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="68">
         <v>36.843596282999997</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="68">
         <v>36.843596282999997</v>
       </c>
       <c r="F9" s="50">
@@ -54391,133 +53972,73 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="52">
-        <v>1</v>
-      </c>
-      <c r="C10" s="52">
-        <v>3</v>
-      </c>
-      <c r="D10" s="52">
-        <v>1</v>
-      </c>
-      <c r="E10" s="52">
-        <v>2</v>
-      </c>
-      <c r="F10" s="52">
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="65">
-        <v>3.4</v>
-      </c>
-      <c r="C11" s="65">
-        <v>3</v>
-      </c>
-      <c r="D11" s="65">
-        <v>2.6</v>
-      </c>
-      <c r="E11" s="65">
-        <v>2.8</v>
-      </c>
-      <c r="F11" s="65">
-        <v>2</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="C12" s="65">
-        <v>3</v>
-      </c>
-      <c r="D12" s="65">
-        <v>2.25</v>
-      </c>
-      <c r="E12" s="65">
-        <v>2.75</v>
-      </c>
-      <c r="F12" s="65">
-        <v>3.5</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="65">
-        <v>2.4</v>
-      </c>
-      <c r="C13" s="65">
-        <v>3.2</v>
-      </c>
-      <c r="D13" s="65">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E13" s="65">
-        <v>3</v>
-      </c>
-      <c r="F13" s="65">
-        <v>4.2</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="65">
-        <v>2</v>
-      </c>
-      <c r="C14" s="65">
-        <v>3.25</v>
-      </c>
-      <c r="D14" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="65">
-        <v>3</v>
-      </c>
-      <c r="F14" s="65">
-        <v>4.25</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="52">
-        <v>1</v>
-      </c>
-      <c r="C15" s="52">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52">
-        <v>1</v>
-      </c>
-      <c r="E15" s="52">
-        <v>2</v>
-      </c>
-      <c r="F15" s="52">
-        <v>5</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="A16" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>

</xml_diff>

<commit_message>
updates, may need to discard or revert
</commit_message>
<xml_diff>
--- a/src/dams_mcda/www/DecisionMatrices_All.xlsx
+++ b/src/dams_mcda/www/DecisionMatrices_All.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20235" windowHeight="7050" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20235" windowHeight="7050" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="10" r:id="rId1"/>
@@ -1293,7 +1293,7 @@
   </sheetPr>
   <dimension ref="A1:AA1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -31062,9 +31062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10:F15"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F15" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31213,16 +31213,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -34303,8 +34303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F15"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34453,16 +34453,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -37543,8 +37543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37693,16 +37693,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -40779,8 +40779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F15"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -40933,16 +40933,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -44019,8 +44019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F15"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44173,16 +44173,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -47260,8 +47260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F15"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -47414,16 +47414,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -50501,8 +50501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F15"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -50655,16 +50655,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="52">
         <v>0</v>
@@ -53741,8 +53741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53895,16 +53895,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>

</xml_diff>

<commit_message>
documents update after pre-survey
</commit_message>
<xml_diff>
--- a/src/dams_mcda/www/DecisionMatrices_All.xlsx
+++ b/src/dams_mcda/www/DecisionMatrices_All.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Medway" sheetId="4" r:id="rId3"/>
     <sheet name="East Millinocket" sheetId="6" r:id="rId4"/>
     <sheet name="Dolby" sheetId="8" r:id="rId5"/>
-    <sheet name="MillinocketQuakish" sheetId="5" r:id="rId6"/>
-    <sheet name="North Twin" sheetId="7" r:id="rId7"/>
+    <sheet name="North Twin" sheetId="7" r:id="rId6"/>
+    <sheet name="MillinocketQuakish" sheetId="5" r:id="rId7"/>
     <sheet name="Millinocket Lake" sheetId="9" r:id="rId8"/>
     <sheet name="Ripogenus" sheetId="2" r:id="rId9"/>
     <sheet name="METADATA" sheetId="1" r:id="rId10"/>
@@ -961,8 +961,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -978,6 +976,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2200,7 +2200,7 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
     </row>
-    <row r="20" spans="1:27" s="40" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" s="40" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>84</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
     </row>
-    <row r="26" spans="1:27" ht="120" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>108</v>
       </c>
@@ -31064,7 +31064,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F15" sqref="B2:F15"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31272,19 +31272,19 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="65">
+      <c r="B9" s="63">
         <f>9612.21085822381/1000</f>
         <v>9.6122108582238113</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="63">
         <f t="shared" ref="C9:E9" si="0">9612.21085822381/1000</f>
         <v>9.6122108582238113</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="63">
         <f t="shared" si="0"/>
         <v>9.6122108582238113</v>
       </c>
-      <c r="E9" s="65">
+      <c r="E9" s="63">
         <f t="shared" si="0"/>
         <v>9.6122108582238113</v>
       </c>
@@ -31296,71 +31296,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1</v>
+      </c>
+      <c r="C10" s="68">
+        <v>4</v>
+      </c>
+      <c r="D10" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="68">
+        <v>4</v>
+      </c>
+      <c r="F10" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>3</v>
+      </c>
+      <c r="C11" s="68">
+        <v>3</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3</v>
+      </c>
+      <c r="E11" s="68">
+        <v>2.6666666669999999</v>
+      </c>
+      <c r="F11" s="68">
+        <v>2.3333333330000001</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>3</v>
+      </c>
+      <c r="C12" s="68">
+        <v>3</v>
+      </c>
+      <c r="D12" s="68">
+        <v>2</v>
+      </c>
+      <c r="E12" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="F12" s="68">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="69">
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="C13" s="68">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="68">
+        <v>2.4</v>
+      </c>
+      <c r="E13" s="68">
+        <v>2.3333333330000001</v>
+      </c>
+      <c r="F13" s="68">
+        <v>4.1666666670000003</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.1666666669999999</v>
+      </c>
+      <c r="C14" s="68">
+        <v>3.8</v>
+      </c>
+      <c r="D14" s="68">
+        <v>3</v>
+      </c>
+      <c r="E14" s="68">
+        <v>3.25</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4.3333333329999997</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="65">
+        <v>1</v>
+      </c>
+      <c r="C15" s="65">
+        <v>4.5</v>
+      </c>
+      <c r="D15" s="65">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="65">
+        <v>4</v>
+      </c>
+      <c r="F15" s="65">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -34303,8 +34363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34512,19 +34572,19 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="66">
+      <c r="B9" s="64">
         <f>5058.83186163302/1000</f>
         <v>5.0588318616330197</v>
       </c>
-      <c r="C9" s="66">
+      <c r="C9" s="64">
         <f>8676.48487896361/1000</f>
         <v>8.6764848789636115</v>
       </c>
-      <c r="D9" s="66">
+      <c r="D9" s="64">
         <f>5058.83186163302/1000</f>
         <v>5.0588318616330197</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="64">
         <f>8676.48487896361/1000</f>
         <v>8.6764848789636115</v>
       </c>
@@ -34536,71 +34596,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1.3333333329999999</v>
+      </c>
+      <c r="C10" s="68">
+        <v>4</v>
+      </c>
+      <c r="D10" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="68">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>2.3333333330000001</v>
+      </c>
+      <c r="C12" s="68">
+        <v>3</v>
+      </c>
+      <c r="D12" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="E12" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="F12" s="68">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>1.4</v>
+      </c>
+      <c r="C13" s="68">
+        <v>3.3333333330000001</v>
+      </c>
+      <c r="D13" s="68">
+        <v>1.6666666670000001</v>
+      </c>
+      <c r="E13" s="68">
+        <v>3</v>
+      </c>
+      <c r="F13" s="68">
+        <v>4.8</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>1.8</v>
+      </c>
+      <c r="C14" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D14" s="68">
+        <v>2</v>
+      </c>
+      <c r="E14" s="68">
+        <v>4</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4.4000000000000004</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="68">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>4</v>
+      </c>
+      <c r="D15" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="68">
+        <v>4</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -37543,8 +37663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37752,16 +37872,16 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="67">
+      <c r="B9" s="65">
         <v>6.782771221</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="65">
         <v>6.782771221</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="66">
         <v>10.756990114000001</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="66">
         <v>10.756990114000001</v>
       </c>
       <c r="F9" s="50">
@@ -37772,71 +37892,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1</v>
+      </c>
+      <c r="C10" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="68">
+        <v>2</v>
+      </c>
+      <c r="E10" s="68">
+        <v>3.875</v>
+      </c>
+      <c r="F10" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>3.3333333330000001</v>
+      </c>
+      <c r="C11" s="68">
+        <v>5</v>
+      </c>
+      <c r="D11" s="68">
+        <v>5</v>
+      </c>
+      <c r="E11" s="68">
+        <v>5</v>
+      </c>
+      <c r="F11" s="68">
+        <v>2.6666666669999999</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C12" s="68">
+        <v>5</v>
+      </c>
+      <c r="D12" s="68">
+        <v>5</v>
+      </c>
+      <c r="E12" s="68">
+        <v>5</v>
+      </c>
+      <c r="F12" s="68">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>2.6666666669999999</v>
+      </c>
+      <c r="C13" s="68">
+        <v>5</v>
+      </c>
+      <c r="D13" s="68">
+        <v>5</v>
+      </c>
+      <c r="E13" s="68">
+        <v>5</v>
+      </c>
+      <c r="F13" s="68">
+        <v>3.3333333330000001</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.6666666669999999</v>
+      </c>
+      <c r="C14" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="D14" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="68">
+        <v>3.6666666669999999</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="68">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>4.375</v>
+      </c>
+      <c r="D15" s="68">
+        <v>2</v>
+      </c>
+      <c r="E15" s="68">
+        <v>3.75</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -40779,8 +40959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -40992,16 +41172,16 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="66">
         <v>12.88193832</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="66">
         <v>12.88193832</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="66">
         <v>12.88193832</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="66">
         <v>12.88193832</v>
       </c>
       <c r="F9" s="50">
@@ -41012,71 +41192,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="68">
+        <v>5</v>
+      </c>
+      <c r="D10" s="68">
+        <v>3</v>
+      </c>
+      <c r="E10" s="68">
+        <v>4</v>
+      </c>
+      <c r="F10" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>3</v>
+      </c>
+      <c r="C11" s="68">
+        <v>3</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="F11" s="68">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>2.6666666669999999</v>
+      </c>
+      <c r="C12" s="68">
+        <v>4</v>
+      </c>
+      <c r="D12" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="E12" s="68">
+        <v>4</v>
+      </c>
+      <c r="F12" s="68">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>2.75</v>
+      </c>
+      <c r="C13" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D13" s="68">
+        <v>4</v>
+      </c>
+      <c r="E13" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="F13" s="68">
+        <v>3.25</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.25</v>
+      </c>
+      <c r="C14" s="68">
+        <v>3.6666666669999999</v>
+      </c>
+      <c r="D14" s="68">
+        <v>3</v>
+      </c>
+      <c r="E14" s="68">
+        <v>3.3333333330000001</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4.25</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="C15" s="68">
+        <v>4</v>
+      </c>
+      <c r="D15" s="68">
+        <v>3</v>
+      </c>
+      <c r="E15" s="68">
+        <v>3</v>
+      </c>
+      <c r="F15" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -44016,11 +44256,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44092,16 +44332,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -44109,19 +44349,19 @@
         <v>23</v>
       </c>
       <c r="B3" s="50">
-        <v>0.29859999999999998</v>
+        <v>1.57</v>
       </c>
       <c r="C3" s="50">
-        <v>0.29859999999999998</v>
+        <v>1.57</v>
       </c>
       <c r="D3" s="50">
-        <v>0.29859999999999998</v>
+        <v>1.57</v>
       </c>
       <c r="E3" s="50">
-        <v>0.29859999999999998</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>149</v>
+        <v>1.57</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -44129,20 +44369,20 @@
         <v>24</v>
       </c>
       <c r="B4" s="54">
-        <f t="shared" ref="B4:E4" si="0">9869/100000</f>
-        <v>9.869E-2</v>
+        <f t="shared" ref="B4:E4" si="0">21456/100000</f>
+        <v>0.21456</v>
       </c>
       <c r="C4" s="54">
         <f t="shared" si="0"/>
-        <v>9.869E-2</v>
+        <v>0.21456</v>
       </c>
       <c r="D4" s="54">
         <f t="shared" si="0"/>
-        <v>9.869E-2</v>
+        <v>0.21456</v>
       </c>
       <c r="E4" s="54">
         <f t="shared" si="0"/>
-        <v>9.869E-2</v>
+        <v>0.21456</v>
       </c>
       <c r="F4" s="55">
         <v>0</v>
@@ -44153,19 +44393,19 @@
         <v>25</v>
       </c>
       <c r="B5" s="50">
-        <v>1657.029</v>
+        <v>402.8</v>
       </c>
       <c r="C5" s="50">
-        <v>1969.8309999999999</v>
+        <v>467.46300000000002</v>
       </c>
       <c r="D5" s="50">
-        <v>1657.029</v>
+        <v>1880.377</v>
       </c>
       <c r="E5" s="50">
-        <v>1969.8309999999999</v>
+        <v>1945.04</v>
       </c>
       <c r="F5" s="50">
-        <v>215.15199999999999</v>
+        <v>212.08799999999999</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -44173,16 +44413,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -44205,7 +44445,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="50">
-        <v>9</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -44213,16 +44453,16 @@
         <v>30</v>
       </c>
       <c r="B8" s="45">
-        <v>203</v>
+        <v>47</v>
       </c>
       <c r="C8" s="45">
-        <v>203</v>
+        <v>47</v>
       </c>
       <c r="D8" s="45">
-        <v>203</v>
+        <v>75</v>
       </c>
       <c r="E8" s="45">
-        <v>203</v>
+        <v>75</v>
       </c>
       <c r="F8" s="50">
         <v>0</v>
@@ -44232,17 +44472,18 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="67">
-        <v>26.69620857</v>
-      </c>
-      <c r="C9" s="67">
-        <v>26.69620857</v>
-      </c>
-      <c r="D9" s="67">
-        <v>26.69620857</v>
-      </c>
-      <c r="E9" s="67">
-        <v>26.69620857</v>
+      <c r="B9" s="66">
+        <f>8.509949038</f>
+        <v>8.5099490380000002</v>
+      </c>
+      <c r="C9" s="66">
+        <v>8.5099490380000002</v>
+      </c>
+      <c r="D9" s="66">
+        <v>13.426482992</v>
+      </c>
+      <c r="E9" s="66">
+        <v>13.426482992</v>
       </c>
       <c r="F9" s="50">
         <v>0</v>
@@ -44252,71 +44493,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="68">
+        <v>5</v>
+      </c>
+      <c r="D10" s="68">
+        <v>2</v>
+      </c>
+      <c r="E10" s="68">
+        <v>4</v>
+      </c>
+      <c r="F10" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>3.3333333330000001</v>
+      </c>
+      <c r="C11" s="68">
+        <v>2</v>
+      </c>
+      <c r="D11" s="68">
+        <v>4</v>
+      </c>
+      <c r="E11" s="68">
+        <v>3</v>
+      </c>
+      <c r="F11" s="68">
+        <v>2.6666666669999999</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>3</v>
+      </c>
+      <c r="C12" s="68">
+        <v>4</v>
+      </c>
+      <c r="D12" s="68">
+        <v>3</v>
+      </c>
+      <c r="E12" s="68">
+        <v>4</v>
+      </c>
+      <c r="F12" s="68">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>1.6666666670000001</v>
+      </c>
+      <c r="C13" s="68">
+        <v>4</v>
+      </c>
+      <c r="D13" s="68">
+        <v>3</v>
+      </c>
+      <c r="E13" s="68">
+        <v>3</v>
+      </c>
+      <c r="F13" s="68">
+        <v>4.3333333329999997</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="68">
+        <v>4</v>
+      </c>
+      <c r="D14" s="68">
+        <v>4</v>
+      </c>
+      <c r="E14" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-    </row>
-    <row r="16" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="B15" s="68">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>5</v>
+      </c>
+      <c r="D15" s="68">
+        <v>2</v>
+      </c>
+      <c r="E15" s="68">
+        <v>4</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -47252,16 +47553,15 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F15" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -47333,16 +47633,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D2" s="52">
         <v>0</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -47350,19 +47650,19 @@
         <v>23</v>
       </c>
       <c r="B3" s="50">
-        <v>1.57</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="C3" s="50">
-        <v>1.57</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="D3" s="50">
-        <v>1.57</v>
+        <v>0.29859999999999998</v>
       </c>
       <c r="E3" s="50">
-        <v>1.57</v>
-      </c>
-      <c r="F3" s="61" t="s">
-        <v>153</v>
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -47370,20 +47670,20 @@
         <v>24</v>
       </c>
       <c r="B4" s="54">
-        <f t="shared" ref="B4:E4" si="0">21456/100000</f>
-        <v>0.21456</v>
+        <f t="shared" ref="B4:E4" si="0">9869/100000</f>
+        <v>9.869E-2</v>
       </c>
       <c r="C4" s="54">
         <f t="shared" si="0"/>
-        <v>0.21456</v>
+        <v>9.869E-2</v>
       </c>
       <c r="D4" s="54">
         <f t="shared" si="0"/>
-        <v>0.21456</v>
+        <v>9.869E-2</v>
       </c>
       <c r="E4" s="54">
         <f t="shared" si="0"/>
-        <v>0.21456</v>
+        <v>9.869E-2</v>
       </c>
       <c r="F4" s="55">
         <v>0</v>
@@ -47394,19 +47694,19 @@
         <v>25</v>
       </c>
       <c r="B5" s="50">
-        <v>402.8</v>
+        <v>1657.029</v>
       </c>
       <c r="C5" s="50">
-        <v>467.46300000000002</v>
+        <v>1969.8309999999999</v>
       </c>
       <c r="D5" s="50">
-        <v>1880.377</v>
+        <v>1657.029</v>
       </c>
       <c r="E5" s="50">
-        <v>1945.04</v>
+        <v>1969.8309999999999</v>
       </c>
       <c r="F5" s="50">
-        <v>212.08799999999999</v>
+        <v>215.15199999999999</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -47414,16 +47714,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="50">
         <v>0</v>
@@ -47446,7 +47746,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="50">
-        <v>589</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -47454,16 +47754,16 @@
         <v>30</v>
       </c>
       <c r="B8" s="45">
-        <v>47</v>
+        <v>203</v>
       </c>
       <c r="C8" s="45">
-        <v>47</v>
+        <v>203</v>
       </c>
       <c r="D8" s="45">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="E8" s="45">
-        <v>75</v>
+        <v>203</v>
       </c>
       <c r="F8" s="50">
         <v>0</v>
@@ -47473,18 +47773,17 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="68">
-        <f>8.509949038</f>
-        <v>8.5099490380000002</v>
-      </c>
-      <c r="C9" s="68">
-        <v>8.5099490380000002</v>
-      </c>
-      <c r="D9" s="68">
-        <v>13.426482992</v>
-      </c>
-      <c r="E9" s="68">
-        <v>13.426482992</v>
+      <c r="B9" s="65">
+        <v>26.69620857</v>
+      </c>
+      <c r="C9" s="65">
+        <v>26.69620857</v>
+      </c>
+      <c r="D9" s="65">
+        <v>26.69620857</v>
+      </c>
+      <c r="E9" s="65">
+        <v>26.69620857</v>
       </c>
       <c r="F9" s="50">
         <v>0</v>
@@ -47494,71 +47793,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1</v>
+      </c>
+      <c r="C10" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="68">
+        <v>2</v>
+      </c>
+      <c r="E10" s="68">
+        <v>3.875</v>
+      </c>
+      <c r="F10" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="68">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="68">
+        <v>3.1333333329999999</v>
+      </c>
+      <c r="F11" s="68">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>1</v>
+      </c>
+      <c r="C12" s="68">
+        <v>3.8</v>
+      </c>
+      <c r="D12" s="68">
+        <v>3</v>
+      </c>
+      <c r="E12" s="68">
+        <v>3.6</v>
+      </c>
+      <c r="F12" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="68">
+        <v>3.2023809519999999</v>
+      </c>
+      <c r="D13" s="68">
+        <v>3.3444444440000001</v>
+      </c>
+      <c r="E13" s="68">
+        <v>3.638888889</v>
+      </c>
+      <c r="F13" s="68">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="68">
+        <v>4</v>
+      </c>
+      <c r="D14" s="68">
+        <v>4</v>
+      </c>
+      <c r="E14" s="68">
+        <v>4</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-    </row>
-    <row r="16" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="B15" s="68">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>4.375</v>
+      </c>
+      <c r="D15" s="68">
+        <v>2</v>
+      </c>
+      <c r="E15" s="68">
+        <v>3.75</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -50494,6 +50853,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -50501,8 +50861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -50720,10 +51080,10 @@
       <c r="C9" s="52">
         <v>0</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="66">
         <v>9.5859479999999997E-2</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="66">
         <v>9.5859479999999997E-2</v>
       </c>
       <c r="F9" s="52">
@@ -50731,74 +51091,134 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1</v>
+      </c>
+      <c r="C10" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="68">
+        <v>2</v>
+      </c>
+      <c r="E10" s="68">
+        <v>3.875</v>
+      </c>
+      <c r="F10" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>2</v>
+      </c>
+      <c r="C11" s="68">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3.5</v>
+      </c>
+      <c r="E11" s="68">
+        <v>3.1333333329999999</v>
+      </c>
+      <c r="F11" s="68">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>1</v>
+      </c>
+      <c r="C12" s="68">
+        <v>3.8</v>
+      </c>
+      <c r="D12" s="68">
+        <v>3</v>
+      </c>
+      <c r="E12" s="68">
+        <v>3.6</v>
+      </c>
+      <c r="F12" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="68">
+        <v>4</v>
+      </c>
+      <c r="D13" s="68">
+        <v>3</v>
+      </c>
+      <c r="E13" s="68">
+        <v>4</v>
+      </c>
+      <c r="F13" s="68">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="68">
+        <v>4</v>
+      </c>
+      <c r="D14" s="68">
+        <v>4</v>
+      </c>
+      <c r="E14" s="68">
+        <v>4</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="68">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>4.375</v>
+      </c>
+      <c r="D15" s="68">
+        <v>2</v>
+      </c>
+      <c r="E15" s="68">
+        <v>3.75</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
@@ -53742,7 +54162,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -53954,16 +54374,16 @@
       <c r="A9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="66">
         <v>30.727559299999999</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="66">
         <v>30.727559299999999</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="66">
         <v>36.843596282999997</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="66">
         <v>36.843596282999997</v>
       </c>
       <c r="F9" s="50">
@@ -53974,71 +54394,131 @@
       <c r="A10" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="68">
+        <v>1</v>
+      </c>
+      <c r="C10" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D10" s="68">
+        <v>2</v>
+      </c>
+      <c r="E10" s="68">
+        <v>3.875</v>
+      </c>
+      <c r="F10" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="68">
+        <v>2</v>
+      </c>
+      <c r="C11" s="68">
+        <v>2.9</v>
+      </c>
+      <c r="D11" s="68">
+        <v>3</v>
+      </c>
+      <c r="E11" s="68">
+        <v>3.1333333329999999</v>
+      </c>
+      <c r="F11" s="68">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="68">
+        <v>1</v>
+      </c>
+      <c r="C12" s="68">
+        <v>3.8</v>
+      </c>
+      <c r="D12" s="68">
+        <v>3</v>
+      </c>
+      <c r="E12" s="68">
+        <v>3.6</v>
+      </c>
+      <c r="F12" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="C13" s="68">
+        <v>3.44047619</v>
+      </c>
+      <c r="D13" s="68">
+        <v>3.3444444440000001</v>
+      </c>
+      <c r="E13" s="68">
+        <v>3.638888889</v>
+      </c>
+      <c r="F13" s="68">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="68">
+        <v>2.5</v>
+      </c>
+      <c r="C14" s="68">
+        <v>4</v>
+      </c>
+      <c r="D14" s="68">
+        <v>4</v>
+      </c>
+      <c r="E14" s="68">
+        <v>4</v>
+      </c>
+      <c r="F14" s="68">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
+      <c r="B15" s="68">
+        <v>1</v>
+      </c>
+      <c r="C15" s="68">
+        <v>4.375</v>
+      </c>
+      <c r="D15" s="68">
+        <v>2</v>
+      </c>
+      <c r="E15" s="68">
+        <v>3.75</v>
+      </c>
+      <c r="F15" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>

</xml_diff>